<commit_message>
Refactored code in BaseTest,LoginTest and added new seachTestModel and test class
</commit_message>
<xml_diff>
--- a/src/main/resources/testNopCommerceData.xlsx
+++ b/src/main/resources/testNopCommerceData.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t>url</t>
   </si>
@@ -75,13 +75,16 @@
     <t>testSearchProduct</t>
   </si>
   <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>Computers</t>
+  </si>
+  <si>
+    <t>testAddProduct</t>
+  </si>
+  <si>
     <t>Asus Laptop</t>
-  </si>
-  <si>
-    <t>Computers</t>
-  </si>
-  <si>
-    <t>testAddProduct</t>
   </si>
   <si>
     <t>testUpdateProduct</t>
@@ -1174,7 +1177,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="3"/>
@@ -1218,7 +1221,7 @@
         <v>17</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C3">
         <v>101</v>
@@ -1229,10 +1232,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4">
         <v>102</v>
@@ -1243,10 +1246,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="C5">
         <v>103</v>

</xml_diff>